<commit_message>
yenı medıan ve anlıyz
</commit_message>
<xml_diff>
--- a/src/algortitma project.xlsx
+++ b/src/algortitma project.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suleyman\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\suleyman\Documents\GitHub\algoProje\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB0ED33-1217-4B8A-BC06-C7D78E943137}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8503F86F-6AC4-4F3F-89E9-0932A601B9BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="384" yWindow="72" windowWidth="10140" windowHeight="12288" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Average" sheetId="1" r:id="rId1"/>
@@ -15768,16 +15768,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>267135</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>174297</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>599962</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>165538</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>376619</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>61310</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>113860</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>52551</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16057,15 +16057,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>538655</xdr:colOff>
-      <xdr:row>132</xdr:row>
-      <xdr:rowOff>183055</xdr:rowOff>
+      <xdr:colOff>286871</xdr:colOff>
+      <xdr:row>131</xdr:row>
+      <xdr:rowOff>121383</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>188310</xdr:colOff>
-      <xdr:row>147</xdr:row>
-      <xdr:rowOff>167290</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>304080</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>71718</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16358,8 +16358,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CK145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView tabSelected="1" topLeftCell="I127" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q131" sqref="Q131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18763,8 +18763,14 @@
       <c r="H16" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="J16" s="5">
+        <v>500</v>
+      </c>
+      <c r="K16" s="2">
+        <v>22026</v>
+      </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>500</v>
       </c>
@@ -18789,8 +18795,14 @@
       <c r="H17" s="2">
         <v>3783</v>
       </c>
+      <c r="J17" s="6">
+        <v>1000</v>
+      </c>
+      <c r="K17" s="2">
+        <v>73742</v>
+      </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="6">
         <v>1000</v>
       </c>
@@ -18815,8 +18827,14 @@
       <c r="H18" s="2">
         <v>3772</v>
       </c>
+      <c r="J18" s="5">
+        <v>2000</v>
+      </c>
+      <c r="K18" s="2">
+        <v>285831</v>
+      </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="5">
         <v>2000</v>
       </c>
@@ -18841,8 +18859,14 @@
       <c r="H19" s="2">
         <v>8662</v>
       </c>
+      <c r="J19" s="6">
+        <v>3000</v>
+      </c>
+      <c r="K19" s="2">
+        <v>640100</v>
+      </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="6">
         <v>3000</v>
       </c>
@@ -18867,8 +18891,14 @@
       <c r="H20" s="2">
         <v>17781</v>
       </c>
+      <c r="J20" s="5">
+        <v>4000</v>
+      </c>
+      <c r="K20" s="2">
+        <v>1140631</v>
+      </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <v>4000</v>
       </c>
@@ -18893,8 +18923,14 @@
       <c r="H21" s="2">
         <v>24090</v>
       </c>
+      <c r="J21" s="6">
+        <v>5000</v>
+      </c>
+      <c r="K21" s="2">
+        <v>1759657</v>
+      </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="6">
         <v>5000</v>
       </c>
@@ -18919,8 +18955,14 @@
       <c r="H22" s="2">
         <v>31213</v>
       </c>
+      <c r="J22" s="5">
+        <v>6000</v>
+      </c>
+      <c r="K22" s="2">
+        <v>2514589</v>
+      </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <v>6000</v>
       </c>
@@ -18945,8 +18987,14 @@
       <c r="H23" s="2">
         <v>37634</v>
       </c>
+      <c r="J23" s="6">
+        <v>7000</v>
+      </c>
+      <c r="K23" s="2">
+        <v>3463290</v>
+      </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="6">
         <v>7000</v>
       </c>
@@ -18971,8 +19019,14 @@
       <c r="H24" s="2">
         <v>41672</v>
       </c>
+      <c r="J24" s="5">
+        <v>8000</v>
+      </c>
+      <c r="K24" s="2">
+        <v>4380130</v>
+      </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <v>8000</v>
       </c>
@@ -18997,8 +19051,14 @@
       <c r="H25" s="2">
         <v>54930</v>
       </c>
+      <c r="J25" s="6">
+        <v>9000</v>
+      </c>
+      <c r="K25" s="2">
+        <v>5521536</v>
+      </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" s="6">
         <v>9000</v>
       </c>
@@ -19023,8 +19083,14 @@
       <c r="H26" s="2">
         <v>54539</v>
       </c>
+      <c r="J26" s="7">
+        <v>10000</v>
+      </c>
+      <c r="K26" s="2">
+        <v>6861524</v>
+      </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="7">
         <v>10000</v>
       </c>
@@ -19050,7 +19116,7 @@
         <v>57526</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -19060,7 +19126,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>2</v>
       </c>
@@ -19073,7 +19139,7 @@
       <c r="H29" s="8"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" s="2"/>
       <c r="B30" s="2" t="s">
         <v>10</v>
@@ -19098,7 +19164,7 @@
       </c>
       <c r="I30" s="4"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>500</v>
       </c>
@@ -19125,7 +19191,7 @@
       </c>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" s="6">
         <v>1000</v>
       </c>

</xml_diff>